<commit_message>
420 + 18 changes
It's nice now
</commit_message>
<xml_diff>
--- a/DOCS/EIGEN/Voortgang.xlsx
+++ b/DOCS/EIGEN/Voortgang.xlsx
@@ -193,14 +193,8 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:C19" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:C19">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Must"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="A2:C19">
+  <autoFilter ref="A1:C19"/>
+  <sortState ref="A2:C11">
     <sortCondition ref="B2:B19" customList="Must,Should,Could,Would"/>
     <sortCondition ref="C2:C19" customList="+,+/-,-"/>
     <sortCondition ref="A2:A19"/>
@@ -480,7 +474,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +497,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
@@ -514,7 +508,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -525,7 +519,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
@@ -536,7 +530,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -547,46 +541,46 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -597,21 +591,21 @@
         <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -622,7 +616,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -633,7 +627,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -644,7 +638,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -655,7 +649,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -666,7 +660,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -677,7 +671,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -688,7 +682,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>

</xml_diff>